<commit_message>
Modified layout/added dynamic filtering
</commit_message>
<xml_diff>
--- a/topMovies.xlsx
+++ b/topMovies.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ae2fb1cdeb1cc68c/Documents/personalGit/movies/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D26F1B42-5E28-44D2-A57B-308BFF480E06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{D26F1B42-5E28-44D2-A57B-308BFF480E06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D4033BAB-0A48-4B8F-A96C-B65877A74E1B}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{68A73E72-3695-456C-B545-507114631371}"/>
+    <workbookView xWindow="3000" yWindow="3000" windowWidth="16920" windowHeight="10450" xr2:uid="{68A73E72-3695-456C-B545-507114631371}"/>
   </bookViews>
   <sheets>
     <sheet name="imdb_top_1000" sheetId="1" r:id="rId1"/>
@@ -19730,7 +19730,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -19861,6 +19861,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -20163,7 +20171,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -20206,11 +20214,13 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -20244,6 +20254,7 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -20587,7 +20598,7 @@
   <dimension ref="A1:L1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -20631,7 +20642,7 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B2" t="s">
@@ -58328,6 +58339,9 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{9E25CE1C-1C49-4A48-9A94-70B4EEC2714C}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added authentication, fixed All Movies display, My List display, made Dashboard template, added Reviews/Rating
</commit_message>
<xml_diff>
--- a/topMovies.xlsx
+++ b/topMovies.xlsx
@@ -20278,6 +20278,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -20597,8 +20601,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09AED6CC-D494-45A1-BFB6-1BFCDEA9F69A}">
   <dimension ref="A1:L1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>